<commit_message>
Add BOOT contract validator + tests + CI gate
Converts BOOT!A1 into an enforced contract with required metadata keys
(version, ttl_hours_default, risk_lane_default, schema_ref, owner).
Adds validator tool, 4 fixture workbooks, 10 tests, and CI gate.
Regenerates template workbook with new BOOT! prefix.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/templates/creative_director_suite/Creative_Director_Suite_CoherenceOps_v2.xlsx
+++ b/templates/creative_director_suite/Creative_Director_Suite_CoherenceOps_v2.xlsx
@@ -617,8 +617,15 @@
   </cols>
   <sheetData>
     <row r="1" ht="800" customHeight="1">
-      <c r="A1" s="1">
-        <f>== CREATIVE DIRECTOR SUITE — COHERENCE OPS WORKBOOK v2.0 ===
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BOOT! METADATA
+version: 0.6.3
+ttl_hours_default: 168
+risk_lane_default: ADVISORY
+schema_ref: docs/excel-first/TABLE_SCHEMAS.md
+owner: Creative Ops Team
+=== CREATIVE DIRECTOR SUITE — COHERENCE OPS WORKBOOK v2.0 ===
 YOU ARE: Creative Ops Copilot (Coherence Ops: Truth · Reasoning · Memory)
 OPENING MOVE:
 1) Read this workbook's tables (tblTimeline, tblDeliverables, tblClaims, tblAssumptions, tblDLR, tblPatchLog, tblCanonGuardrails).
@@ -655,11 +662,11 @@
 NAMED TABLES:
 tblTimeline, tblDeliverables, tblDLR, tblClaims, tblAssumptions, tblPatchLog, tblCanonGuardrails
 PROVENANCE:
-Generated by: DeepSigma v0.6.2 — tools/generate_cds_workbook.py
+Generated by: DeepSigma v0.6.3 — tools/generate_cds_workbook.py
 Framework: Σ OVERWATCH Coherence Ops
 Date: 2026-02-19
-</f>
-        <v/>
+</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>